<commit_message>
Aktualizacja plików (baza zawodow)
</commit_message>
<xml_diff>
--- a/build/app/intermediates/assets/debug/flutter_assets/pliki_bazy/polecane.xlsx
+++ b/build/app/intermediates/assets/debug/flutter_assets/pliki_bazy/polecane.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\kiedy_biegam\app_kb\pliki_bazy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA59231D-DA1E-46DA-97A5-B4AA2167FE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A54EAC1-4727-4D35-B593-DF81EC984726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29625" yWindow="2880" windowWidth="20595" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="240" windowWidth="19620" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>10. Łańcucka Piętka</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 km </t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>https://runrzeszow.pl/zapisy/polmaraton/</t>
+  </si>
+  <si>
+    <t>10. Łańcucka Piątka</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,42 +425,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>45899</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>45814</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>